<commit_message>
Update la lista cu temelerepartizate mti2
</commit_message>
<xml_diff>
--- a/mti2-repartizarea-temelor-2021.xlsx
+++ b/mti2-repartizarea-temelor-2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axa\Documents\Reps\andrei-rusu-ovidius.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E583A5-1C7D-48C7-808E-2A10C982EEBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850310B9-F2D3-41E0-9D7C-A4BDD125E46F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48A4725A-5667-4701-8404-34D3F26A8004}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,6 +544,12 @@
         <v>26</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <f>COUNTA(D5:D20)</f>
+        <v>9</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
@@ -640,9 +646,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
@@ -706,7 +710,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -714,7 +718,9 @@
         <v>29</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.35">
       <c r="A19" s="1">

</xml_diff>

<commit_message>
.xlscu teme la mti2
</commit_message>
<xml_diff>
--- a/mti2-repartizarea-temelor-2021.xlsx
+++ b/mti2-repartizarea-temelor-2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axa\Documents\Reps\andrei-rusu-ovidius.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850310B9-F2D3-41E0-9D7C-A4BDD125E46F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF8F39E-4D18-4697-9292-CC61F7B3F6F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48A4725A-5667-4701-8404-34D3F26A8004}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">2.          Consideram o variantă a problemei rucsacului. Fie avem un rucsac in care trebuie sa punem unele obiecte. Forta noastra fiind limitata, nu putem duce mai mult de G kilograme. Și volumul rucsacului V este limitat. Este clar ca nu putem lua toate lucrurile cu noi. Atunci vom considera ca unele lucruri sunt mai importante/utile decât altele. Scopul este de a maximiza utilitatea sumară a obiectelor puse în rucsac. // //. – 4-5 metode diferite pot fi utilizate. </t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>15.     Problema alocării de resurse în spațiu și în timp în anume condiții: problema orarului de muncă - avem consultanți specializați pe anumite probleme, avem clienți care au de rezolvat probleme, fiecare consultant nu poate lucra cu mai mult de 5 clienți la o anumită categorie de probleme. Se dorește de optimizat timpul necesar pentru a asigura consultarea tuturor clienților. Evident, că atât clienții, cât și consultanții au și ei restricțiile lor ce țin de întâlniri.</t>
+  </si>
+  <si>
+    <t>mi-a aratat</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37686383-87C6-4710-8DDE-93F68A7F4530}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,7 +703,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" ht="117" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="117" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -710,7 +713,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -721,8 +724,11 @@
       <c r="D18" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.35">
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="78" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -734,7 +740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Modificare alocare tema mti2
</commit_message>
<xml_diff>
--- a/mti2-repartizarea-temelor-2021.xlsx
+++ b/mti2-repartizarea-temelor-2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axa\Documents\Reps\andrei-rusu-ovidius.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF8F39E-4D18-4697-9292-CC61F7B3F6F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171EFA43-3B49-407E-8240-32A2783ECC40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48A4725A-5667-4701-8404-34D3F26A8004}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37686383-87C6-4710-8DDE-93F68A7F4530}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,9 +613,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
@@ -679,7 +677,9 @@
         <v>8</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1">

</xml_diff>